<commit_message>
FEAT #2134 add var for contacts_v2
</commit_message>
<xml_diff>
--- a/templates/trunk/templates/styles/office/spreadsheet.xlsx
+++ b/templates/trunk/templates/styles/office/spreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>NAME</t>
   </si>
@@ -24,33 +24,15 @@
     <t>VAR</t>
   </si>
   <si>
-    <t>Contact externe: Civilité</t>
-  </si>
-  <si>
-    <t>Contact externe: Nom</t>
-  </si>
-  <si>
-    <t>Contact externe: Prénom</t>
-  </si>
-  <si>
-    <t>Contact externe : Organisation</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse N°</t>
   </si>
   <si>
     <t>Contact externe : Adresse Rue</t>
   </si>
   <si>
-    <t>Contact externe : Adresse Complement</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Ville</t>
   </si>
   <si>
-    <t>Contact externe : Adresse CP</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Pays</t>
   </si>
   <si>
@@ -202,6 +184,108 @@
   </si>
   <si>
     <t>[attachments.chrono]</t>
+  </si>
+  <si>
+    <t>Contact externe : Type de contact</t>
+  </si>
+  <si>
+    <t>[contact.contact_type_label]</t>
+  </si>
+  <si>
+    <t>Contact externe : Structure</t>
+  </si>
+  <si>
+    <t>Contact externe : Sigle de la structure</t>
+  </si>
+  <si>
+    <t>[contact.society_short]</t>
+  </si>
+  <si>
+    <t>Contact externes : nom du contact</t>
+  </si>
+  <si>
+    <t>[contact.contact_lastname]</t>
+  </si>
+  <si>
+    <t>Contact externes : prénom du contact</t>
+  </si>
+  <si>
+    <t>[contact.contact_firstname]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Dénomination</t>
+  </si>
+  <si>
+    <t>[contact.contact_purpose_label]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Service</t>
+  </si>
+  <si>
+    <t>[contact.departement]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Civilité</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Nom</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Prénom</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Fonction</t>
+  </si>
+  <si>
+    <t>[contact.function]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Etage, bureau, porte</t>
+  </si>
+  <si>
+    <t>[contact.occupancy]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Complément</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Code Postal</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Téléphone</t>
+  </si>
+  <si>
+    <t>[contact.phone]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Courriel</t>
+  </si>
+  <si>
+    <t>[contact.email]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Site internet</t>
+  </si>
+  <si>
+    <t>[contact.website]</t>
+  </si>
+  <si>
+    <t>Contact externe : Formule de politesse de début de courrier</t>
+  </si>
+  <si>
+    <t>[contact.salutation_header]</t>
+  </si>
+  <si>
+    <t>Contact externe : Formule de politesse de fin de courrier</t>
+  </si>
+  <si>
+    <t>[contact.salutation_footer]</t>
+  </si>
+  <si>
+    <t>Courrier : Service initiateur</t>
+  </si>
+  <si>
+    <t>[res_letterbox.initiator]</t>
   </si>
 </sst>
 </file>
@@ -248,6 +332,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -296,7 +383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,7 +418,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,19 +627,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,256 +648,369 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -819,7 +1020,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -831,7 +1032,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FEAT #2134 ajouter balise pour code barres chrono
</commit_message>
<xml_diff>
--- a/templates/trunk/templates/styles/office/spreadsheet.xlsx
+++ b/templates/trunk/templates/styles/office/spreadsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>NAME</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>[res_letterbox.initiator]</t>
+  </si>
+  <si>
+    <t>[attachments.chronoBarCode;ope=changepic]</t>
+  </si>
+  <si>
+    <t>Insérer une image juste au dessus de cette balise</t>
   </si>
 </sst>
 </file>
@@ -627,15 +633,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
@@ -1006,6 +1012,14 @@
       </c>
       <c r="B46" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>